<commit_message>
ECEN301 lab 2 report complete
</commit_message>
<xml_diff>
--- a/2020/RESE412/Project_1/data/week_data.xlsx
+++ b/2020/RESE412/Project_1/data/week_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\uni\2020\RESE412\Project_1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{24E6FC07-4CA2-4D17-9AE5-145AE4577881}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466C4F7B-3FE1-4B8F-AF7C-71ABA061F6BF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32295" yWindow="8445" windowWidth="19305" windowHeight="11505" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resource_data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>NIWA SolarView Calculations</t>
   </si>
@@ -109,11 +109,26 @@
   <si>
     <t>daily usage (kWh)</t>
   </si>
+  <si>
+    <t>$/W</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>$/Ahr</t>
+  </si>
+  <si>
+    <t>Peak Hrs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -966,11 +981,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J182"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5008,62 +5023,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="2:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>17.95</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+        <v>17.88</v>
+      </c>
+      <c r="D3">
+        <v>2.1488571429999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="10">
-        <v>19.86</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+        <v>19.78</v>
+      </c>
+      <c r="D4">
+        <v>2.1488571429999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>15.67</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>2.1488571429999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>39.049999999999997</v>
+        <v>39.590000000000003</v>
+      </c>
+      <c r="D6">
+        <v>2.1488571429999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <v>5.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RESE Proj 1 done
</commit_message>
<xml_diff>
--- a/2020/RESE412/Project_1/data/week_data.xlsx
+++ b/2020/RESE412/Project_1/data/week_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\uni\2020\RESE412\Project_1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA8308F-5939-4EBA-86ED-53E791ED7D6E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4412E1B5-E07E-4247-A314-37DAB4ADD295}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>NIWA SolarView Calculations</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Distributed</t>
   </si>
   <si>
-    <t>Microgrids</t>
-  </si>
-  <si>
     <t>house 2</t>
   </si>
   <si>
@@ -197,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +342,15 @@
       <i/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -692,7 +698,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="18" applyFont="1"/>
@@ -711,10 +717,6 @@
     <xf numFmtId="0" fontId="19" fillId="17" borderId="0" xfId="26" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="26" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="26" applyAlignment="1"/>
     <xf numFmtId="44" fontId="6" fillId="2" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="8" fillId="4" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="7" fillId="3" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
@@ -725,7 +727,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="28" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" xfId="28" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" xfId="28" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8198,10 +8203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:M37"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8216,6 +8221,7 @@
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" customWidth="1"/>
     <col min="13" max="13" width="9.140625" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" customWidth="1"/>
@@ -8313,7 +8319,7 @@
         <f>B8/C8</f>
         <v>8.3207020337507842</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <f>(D8*1000)*B$3</f>
         <v>21633.825287752039</v>
       </c>
@@ -8321,11 +8327,11 @@
         <f>(B8*1000)/240</f>
         <v>74.5</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="16">
         <f>(F8*D$2)*2</f>
         <v>834.4</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="16">
         <f>SUM(E8,G8)</f>
         <v>22468.22528775204</v>
       </c>
@@ -8347,7 +8353,7 @@
         <f t="shared" ref="D9:D11" si="0">B9/C9</f>
         <v>9.2048929657489111</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <f t="shared" ref="E9:E11" si="1">(D9*1000)*B$3</f>
         <v>23932.721710947171</v>
       </c>
@@ -8355,11 +8361,11 @@
         <f>(B9*1000)/240</f>
         <v>82.416666666666671</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="17">
         <f>(F9*D$2)*2</f>
         <v>923.06666666666661</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="17">
         <f t="shared" ref="H9:H11" si="2">SUM(E9,G9)</f>
         <v>24855.788377613837</v>
       </c>
@@ -8381,7 +8387,7 @@
         <f t="shared" si="0"/>
         <v>7.4458183747210605</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="18">
         <f t="shared" si="1"/>
         <v>19359.127774274759</v>
       </c>
@@ -8389,11 +8395,11 @@
         <f>(B10*1000)/240</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="18">
         <f>(F10*D$2)*2</f>
         <v>746.66666666666663</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="18">
         <f t="shared" si="2"/>
         <v>20105.794440941427</v>
       </c>
@@ -8415,7 +8421,7 @@
         <f t="shared" si="0"/>
         <v>18.423746840950425</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="19">
         <f t="shared" si="1"/>
         <v>47901.74178647111</v>
       </c>
@@ -8423,11 +8429,11 @@
         <f>(B11*1000)/240</f>
         <v>164.95833333333334</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="19">
         <f>(F11*D$2)*2</f>
         <v>1847.5333333333333</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="19">
         <f t="shared" si="2"/>
         <v>49749.275119804443</v>
       </c>
@@ -8436,7 +8442,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="22"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
@@ -8494,7 +8500,7 @@
         <f>B16/C16</f>
         <v>1.8944089507644384</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="16">
         <f>(D16*1000)*B$2</f>
         <v>12578.875433075871</v>
       </c>
@@ -8502,11 +8508,11 @@
         <f>(B16*1000)/240</f>
         <v>74.5</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="16">
         <f t="shared" ref="G16:G18" si="3">(F16*D$2)*2</f>
         <v>834.4</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="16">
         <f>SUM(E16,G16)</f>
         <v>13413.275433075871</v>
       </c>
@@ -8514,7 +8520,7 @@
         <v>4.6719999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>3</v>
       </c>
@@ -8528,7 +8534,7 @@
         <f t="shared" ref="D17:D19" si="4">B17/C17</f>
         <v>2.09571638960406</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="17">
         <f>(D17*1000)*B$2</f>
         <v>13915.556826970958</v>
       </c>
@@ -8536,11 +8542,11 @@
         <f>(B17*1000)/240</f>
         <v>82.416666666666671</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="17">
         <f t="shared" si="3"/>
         <v>923.06666666666661</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="17">
         <f>SUM(E17,G17)</f>
         <v>14838.623493637624</v>
       </c>
@@ -8548,7 +8554,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>4</v>
       </c>
@@ -8562,7 +8568,7 @@
         <f t="shared" si="4"/>
         <v>1.695220537596813</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="18">
         <f>(D18*1000)*B$2</f>
         <v>11256.264369642839</v>
       </c>
@@ -8570,11 +8576,11 @@
         <f>(B18*1000)/240</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="18">
         <f t="shared" si="3"/>
         <v>746.66666666666663</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="18">
         <f>SUM(E18,G18)</f>
         <v>12002.931036309505</v>
       </c>
@@ -8582,7 +8588,7 @@
         <v>7.9059999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>5</v>
       </c>
@@ -8596,7 +8602,7 @@
         <f t="shared" si="4"/>
         <v>4.1946113177161148</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="19">
         <f>(D19*1000)*B$2</f>
         <v>27852.219149635002</v>
       </c>
@@ -8604,11 +8610,11 @@
         <f>(B19*1000)/240</f>
         <v>164.95833333333334</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="19">
         <f>(F19*D$2)*2</f>
         <v>1847.5333333333333</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="19">
         <f>SUM(E19,G19)</f>
         <v>29699.752482968335</v>
       </c>
@@ -8616,7 +8622,7 @@
         <v>2.5960000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>44</v>
       </c>
@@ -8629,7 +8635,7 @@
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -8658,7 +8664,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>2</v>
       </c>
@@ -8671,18 +8677,18 @@
       <c r="D25" s="9">
         <v>10</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="16">
         <f>(D25*1000)*B$3</f>
         <v>26000</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="21">
         <v>95</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="16">
         <f>(F25*D$2)*2</f>
         <v>1064</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="16">
         <f>SUM(E25,G25)</f>
         <v>27064</v>
       </c>
@@ -8690,7 +8696,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>3</v>
       </c>
@@ -8703,18 +8709,18 @@
       <c r="D26" s="10">
         <v>12</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="17">
         <f>(D26*1000)*B$3</f>
         <v>31200</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="22">
         <v>100</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="17">
         <f>(F26*D$2)*2</f>
         <v>1120</v>
       </c>
-      <c r="H26" s="19">
+      <c r="H26" s="17">
         <f t="shared" ref="H26:H28" si="5">SUM(E26,G26)</f>
         <v>32320</v>
       </c>
@@ -8722,7 +8728,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>4</v>
       </c>
@@ -8735,18 +8741,18 @@
       <c r="D27" s="12">
         <v>10</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="18">
         <f>(D27*1000)*B$3</f>
         <v>26000</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="23">
         <v>85</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G27" s="18">
         <f>(F27*D$2)*2</f>
         <v>951.99999999999989</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H27" s="18">
         <f t="shared" si="5"/>
         <v>26952</v>
       </c>
@@ -8754,7 +8760,7 @@
         <v>3.64</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>5</v>
       </c>
@@ -8767,26 +8773,30 @@
       <c r="D28" s="13">
         <v>20</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="19">
         <f>(D28*1000)*B$3</f>
         <v>52000</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="24">
         <v>180</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="19">
         <f>(F28*D$2)*2</f>
         <v>2015.9999999999998</v>
       </c>
-      <c r="H28" s="21">
+      <c r="H28" s="19">
         <f t="shared" si="5"/>
         <v>54016</v>
       </c>
       <c r="I28" s="13">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K28" s="25">
+        <f>SUM(H25:H28)</f>
+        <v>140352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>45</v>
       </c>
@@ -8799,7 +8809,7 @@
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -8841,18 +8851,18 @@
       <c r="D33" s="9">
         <v>2</v>
       </c>
-      <c r="E33" s="18">
+      <c r="E33" s="16">
         <f>(D33*1000)*B$2</f>
         <v>13280</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="21">
         <v>80</v>
       </c>
-      <c r="G33" s="18">
+      <c r="G33" s="16">
         <f>(F33*D$2)*2</f>
         <v>896</v>
       </c>
-      <c r="H33" s="18">
+      <c r="H33" s="16">
         <f>SUM(E33,G33)</f>
         <v>14176</v>
       </c>
@@ -8873,18 +8883,18 @@
       <c r="D34" s="10">
         <v>2.6</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="17">
         <f>(D34*1000)*B$2</f>
         <v>17264</v>
       </c>
-      <c r="F34" s="24">
+      <c r="F34" s="22">
         <v>95</v>
       </c>
-      <c r="G34" s="19">
+      <c r="G34" s="17">
         <f>(F34*D$2)*2</f>
         <v>1064</v>
       </c>
-      <c r="H34" s="19">
+      <c r="H34" s="17">
         <f>SUM(E34,G34)</f>
         <v>18328</v>
       </c>
@@ -8905,18 +8915,18 @@
       <c r="D35" s="12">
         <v>1.8</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E35" s="18">
         <f>(D35*1000)*B$2</f>
         <v>11952</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="23">
         <v>85</v>
       </c>
-      <c r="G35" s="20">
+      <c r="G35" s="18">
         <f>(F35*D$2)*2</f>
         <v>951.99999999999989</v>
       </c>
-      <c r="H35" s="20">
+      <c r="H35" s="18">
         <f>SUM(E35,G35)</f>
         <v>12904</v>
       </c>
@@ -8937,54 +8947,43 @@
       <c r="D36" s="13">
         <v>4.5</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="19">
         <f>(D36*1000)*B$2</f>
         <v>29880</v>
       </c>
-      <c r="F36" s="26">
+      <c r="F36" s="24">
         <v>165</v>
       </c>
-      <c r="G36" s="21">
+      <c r="G36" s="19">
         <f>(F36*D$2)*2</f>
         <v>1847.9999999999998</v>
       </c>
-      <c r="H36" s="21">
+      <c r="H36" s="19">
         <f>SUM(E36,G36)</f>
         <v>31728</v>
       </c>
       <c r="I36" s="13">
         <v>1.79</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
+      <c r="K36" s="25">
+        <f>SUM(H33:H36)</f>
+        <v>77136</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -9009,16 +9008,16 @@
         <v>43</v>
       </c>
       <c r="H43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -9030,7 +9029,7 @@
         <f>SUM(D33:D36)</f>
         <v>10.899999999999999</v>
       </c>
-      <c r="C44" s="22">
+      <c r="C44" s="20">
         <f>(B44*1000)*B$2</f>
         <v>72375.999999999985</v>
       </c>
@@ -9038,11 +9037,11 @@
         <f>SUM(F33:F36)</f>
         <v>425</v>
       </c>
-      <c r="E44" s="22">
+      <c r="E44" s="20">
         <f>(D44*D$2)*2</f>
         <v>4760</v>
       </c>
-      <c r="F44" s="22">
+      <c r="F44" s="20">
         <f>SUM(C44,E44)</f>
         <v>77135.999999999985</v>
       </c>
@@ -9064,46 +9063,68 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>88.75</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>10</v>
       </c>
-      <c r="C46" s="22">
-        <f t="shared" ref="C45:C46" si="6">(B46*1000)*B$2</f>
+      <c r="C47" s="20">
+        <f>(B47*1000)*B$2</f>
         <v>66400</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <v>400</v>
       </c>
-      <c r="E46" s="22">
-        <f t="shared" ref="E45:E46" si="7">(D46*D$2)*2</f>
+      <c r="E47" s="20">
+        <f>(D47*D$2)*2</f>
         <v>4480</v>
       </c>
-      <c r="F46" s="27">
-        <f>SUM(C46,E46)</f>
+      <c r="F47" s="25">
+        <f>SUM(C47,E47)</f>
         <v>70880</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <v>1.982</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="A45:G45"/>
-    <mergeCell ref="F41:K41"/>
     <mergeCell ref="A42:K42"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A14:I14"/>

</xml_diff>